<commit_message>
add prolificid in rank to use in binary
</commit_message>
<xml_diff>
--- a/_static/global/rankrankings/workers_rank_mat.xlsx
+++ b/_static/global/rankrankings/workers_rank_mat.xlsx
@@ -46,27 +46,27 @@
     <t>Jewel</t>
   </si>
   <si>
+    <t>Khushi</t>
+  </si>
+  <si>
     <t>Bri</t>
   </si>
   <si>
-    <t>Khushi</t>
+    <t>Shadaisia</t>
+  </si>
+  <si>
+    <t>Kellie</t>
   </si>
   <si>
     <t>Shaniek</t>
   </si>
   <si>
-    <t>Shadaisia</t>
-  </si>
-  <si>
-    <t>Kellie</t>
+    <t>Lori</t>
   </si>
   <si>
     <t>Tina</t>
   </si>
   <si>
-    <t>Lori</t>
-  </si>
-  <si>
     <t>Giana</t>
   </si>
   <si>
@@ -91,13 +91,13 @@
     <t>Drew</t>
   </si>
   <si>
+    <t>Brennan</t>
+  </si>
+  <si>
+    <t>Jamarii</t>
+  </si>
+  <si>
     <t>Matthew</t>
-  </si>
-  <si>
-    <t>Brennan</t>
-  </si>
-  <si>
-    <t>Jamarii</t>
   </si>
   <si>
     <t>Myles</t>
@@ -528,7 +528,7 @@
         <v>31</v>
       </c>
       <c r="F2">
-        <v>13.36634985893487</v>
+        <v>13.41179440177212</v>
       </c>
       <c r="G2" t="s">
         <v>33</v>
@@ -554,7 +554,7 @@
         <v>31</v>
       </c>
       <c r="F3">
-        <v>13.17384225672477</v>
+        <v>13.28345529631224</v>
       </c>
       <c r="G3" t="s">
         <v>34</v>
@@ -580,7 +580,7 @@
         <v>31</v>
       </c>
       <c r="F4">
-        <v>8.435522967461472</v>
+        <v>8.23763560135623</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
@@ -597,7 +597,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -606,10 +606,10 @@
         <v>31</v>
       </c>
       <c r="F5">
-        <v>8.34383967621485</v>
+        <v>8.166612813012238</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -623,7 +623,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -632,10 +632,10 @@
         <v>31</v>
       </c>
       <c r="F6">
-        <v>8.278735030595699</v>
+        <v>8.005597717419404</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -649,7 +649,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -658,7 +658,7 @@
         <v>31</v>
       </c>
       <c r="F7">
-        <v>5.435857524273124</v>
+        <v>5.361927025870195</v>
       </c>
       <c r="G7" t="s">
         <v>35</v>
@@ -675,7 +675,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -684,10 +684,10 @@
         <v>31</v>
       </c>
       <c r="F8">
-        <v>5.192148305431918</v>
+        <v>5.237683582040133</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H8">
         <v>7</v>
@@ -701,7 +701,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -710,10 +710,10 @@
         <v>31</v>
       </c>
       <c r="F9">
-        <v>5.114808149099144</v>
+        <v>5.010962683506764</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H9">
         <v>8</v>
@@ -727,7 +727,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -736,7 +736,7 @@
         <v>31</v>
       </c>
       <c r="F10">
-        <v>4.127572857403828</v>
+        <v>4.477479880056773</v>
       </c>
       <c r="G10" t="s">
         <v>33</v>
@@ -753,7 +753,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
@@ -762,7 +762,7 @@
         <v>31</v>
       </c>
       <c r="F11">
-        <v>4.076664184514845</v>
+        <v>4.389849861394186</v>
       </c>
       <c r="G11" t="s">
         <v>33</v>
@@ -788,7 +788,7 @@
         <v>31</v>
       </c>
       <c r="F12">
-        <v>2.239981183095495</v>
+        <v>2.382527936458554</v>
       </c>
       <c r="G12" t="s">
         <v>33</v>
@@ -814,7 +814,7 @@
         <v>31</v>
       </c>
       <c r="F13">
-        <v>1.379916767955251</v>
+        <v>1.029173221199296</v>
       </c>
       <c r="G13" t="s">
         <v>34</v>
@@ -840,7 +840,7 @@
         <v>32</v>
       </c>
       <c r="F14">
-        <v>14.13193457363825</v>
+        <v>14.2745467615059</v>
       </c>
       <c r="G14" t="s">
         <v>33</v>
@@ -866,7 +866,7 @@
         <v>32</v>
       </c>
       <c r="F15">
-        <v>13.24852036377619</v>
+        <v>13.07194186949775</v>
       </c>
       <c r="G15" t="s">
         <v>35</v>
@@ -892,7 +892,7 @@
         <v>32</v>
       </c>
       <c r="F16">
-        <v>8.019993989997438</v>
+        <v>8.189927172263737</v>
       </c>
       <c r="G16" t="s">
         <v>35</v>
@@ -918,7 +918,7 @@
         <v>32</v>
       </c>
       <c r="F17">
-        <v>7.17488654104628</v>
+        <v>7.39607034879652</v>
       </c>
       <c r="G17" t="s">
         <v>36</v>
@@ -944,7 +944,7 @@
         <v>32</v>
       </c>
       <c r="F18">
-        <v>6.126027957762686</v>
+        <v>6.323612713011084</v>
       </c>
       <c r="G18" t="s">
         <v>33</v>
@@ -970,7 +970,7 @@
         <v>32</v>
       </c>
       <c r="F19">
-        <v>6.047255851061288</v>
+        <v>6.252130279629233</v>
       </c>
       <c r="G19" t="s">
         <v>33</v>
@@ -987,7 +987,7 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
@@ -996,7 +996,7 @@
         <v>32</v>
       </c>
       <c r="F20">
-        <v>5.369492967572572</v>
+        <v>5.331365905335693</v>
       </c>
       <c r="G20" t="s">
         <v>33</v>
@@ -1013,7 +1013,7 @@
         <v>7</v>
       </c>
       <c r="C21">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
         <v>26</v>
@@ -1022,10 +1022,10 @@
         <v>32</v>
       </c>
       <c r="F21">
-        <v>5.165260742633402</v>
+        <v>5.299930968965304</v>
       </c>
       <c r="G21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H21">
         <v>8</v>
@@ -1039,7 +1039,7 @@
         <v>8</v>
       </c>
       <c r="C22">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
@@ -1048,10 +1048,10 @@
         <v>32</v>
       </c>
       <c r="F22">
-        <v>5.046126320341567</v>
+        <v>5.024612660958182</v>
       </c>
       <c r="G22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H22">
         <v>9</v>
@@ -1074,7 +1074,7 @@
         <v>32</v>
       </c>
       <c r="F23">
-        <v>3.453319444307983</v>
+        <v>3.207723512647401</v>
       </c>
       <c r="G23" t="s">
         <v>35</v>
@@ -1100,7 +1100,7 @@
         <v>32</v>
       </c>
       <c r="F24">
-        <v>1.138808340842022</v>
+        <v>1.345698146888841</v>
       </c>
       <c r="G24" t="s">
         <v>34</v>
@@ -1126,7 +1126,7 @@
         <v>32</v>
       </c>
       <c r="F25">
-        <v>0.1517588624201327</v>
+        <v>0.1471275131748038</v>
       </c>
       <c r="G25" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Hispanics (H) Asians (A)
</commit_message>
<xml_diff>
--- a/_static/global/rankrankings/workers_rank_mat.xlsx
+++ b/_static/global/rankrankings/workers_rank_mat.xlsx
@@ -43,24 +43,24 @@
     <t>5c27de12a2b00a00018b2c16</t>
   </si>
   <si>
+    <t>60b1742bce2b39e0f1d19a1a</t>
+  </si>
+  <si>
     <t>60bd88b8fc436774352f53b9</t>
   </si>
   <si>
     <t>5f2c1a97a6809c060fec8820</t>
   </si>
   <si>
-    <t>60b1742bce2b39e0f1d19a1a</t>
-  </si>
-  <si>
     <t>5f7cbf8a2fe61814cae2ce8b</t>
   </si>
   <si>
+    <t>60b7cd4be2d4cc6bb252e016</t>
+  </si>
+  <si>
     <t>5ff3974450a7199965624df7</t>
   </si>
   <si>
-    <t>60b7cd4be2d4cc6bb252e016</t>
-  </si>
-  <si>
     <t>60a71d27a66fac796ad4de6f</t>
   </si>
   <si>
@@ -94,45 +94,45 @@
     <t>5dd671942b033b5ec8bc97b4</t>
   </si>
   <si>
+    <t>6024c18b094ac71dd93f4f5a</t>
+  </si>
+  <si>
     <t>5e35d91ea42bce592e996843</t>
   </si>
   <si>
     <t>5f0142aa1eb1e528e7abce50</t>
   </si>
   <si>
-    <t>6024c18b094ac71dd93f4f5a</t>
-  </si>
-  <si>
     <t>60743a8fd12c5ffa72972fd5</t>
   </si>
   <si>
+    <t>5e58b3e415b8d40b5e1dabf1</t>
+  </si>
+  <si>
     <t>5f5ea8227fa75676f56f9276</t>
   </si>
   <si>
-    <t>5e58b3e415b8d40b5e1dabf1</t>
-  </si>
-  <si>
     <t>Ankai</t>
   </si>
   <si>
+    <t>Sabrina</t>
+  </si>
+  <si>
     <t>Annes</t>
   </si>
   <si>
     <t>Maggie</t>
   </si>
   <si>
-    <t>Sabrina</t>
-  </si>
-  <si>
     <t>Aalap</t>
   </si>
   <si>
+    <t>Chris</t>
+  </si>
+  <si>
     <t>Anh</t>
   </si>
   <si>
-    <t>Chris</t>
-  </si>
-  <si>
     <t>Jennifer</t>
   </si>
   <si>
@@ -166,22 +166,22 @@
     <t>Juan</t>
   </si>
   <si>
+    <t>Katherine</t>
+  </si>
+  <si>
     <t>Sergio</t>
   </si>
   <si>
     <t>Valeria</t>
   </si>
   <si>
-    <t>Katherine</t>
-  </si>
-  <si>
     <t>Josue</t>
   </si>
   <si>
+    <t>Cristian</t>
+  </si>
+  <si>
     <t>Carlos</t>
-  </si>
-  <si>
-    <t>Cristian</t>
   </si>
   <si>
     <t>male</t>
@@ -603,7 +603,7 @@
         <v>56</v>
       </c>
       <c r="G2">
-        <v>14.36489732955242</v>
+        <v>14.39815288238974</v>
       </c>
       <c r="H2" t="s">
         <v>58</v>
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -632,7 +632,7 @@
         <v>57</v>
       </c>
       <c r="G3">
-        <v>13.45093157762697</v>
+        <v>13.47099616876117</v>
       </c>
       <c r="H3" t="s">
         <v>58</v>
@@ -649,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -661,7 +661,7 @@
         <v>57</v>
       </c>
       <c r="G4">
-        <v>13.24590183972602</v>
+        <v>13.17858138422446</v>
       </c>
       <c r="H4" t="s">
         <v>58</v>
@@ -678,7 +678,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -690,7 +690,7 @@
         <v>57</v>
       </c>
       <c r="G5">
-        <v>13.16029971904301</v>
+        <v>13.01112575673547</v>
       </c>
       <c r="H5" t="s">
         <v>58</v>
@@ -719,7 +719,7 @@
         <v>56</v>
       </c>
       <c r="G6">
-        <v>12.247818214573</v>
+        <v>12.3482248776141</v>
       </c>
       <c r="H6" t="s">
         <v>58</v>
@@ -736,7 +736,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -748,7 +748,7 @@
         <v>56</v>
       </c>
       <c r="G7">
-        <v>10.30328183410595</v>
+        <v>10.34214312864992</v>
       </c>
       <c r="H7" t="s">
         <v>58</v>
@@ -765,7 +765,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -777,7 +777,7 @@
         <v>56</v>
       </c>
       <c r="G8">
-        <v>10.17991156201473</v>
+        <v>10.06224892236708</v>
       </c>
       <c r="H8" t="s">
         <v>58</v>
@@ -806,7 +806,7 @@
         <v>57</v>
       </c>
       <c r="G9">
-        <v>8.424071716781192</v>
+        <v>8.014854919004936</v>
       </c>
       <c r="H9" t="s">
         <v>58</v>
@@ -835,7 +835,7 @@
         <v>56</v>
       </c>
       <c r="G10">
-        <v>5.018050929083364</v>
+        <v>5.498532721451911</v>
       </c>
       <c r="H10" t="s">
         <v>58</v>
@@ -864,7 +864,7 @@
         <v>56</v>
       </c>
       <c r="G11">
-        <v>2.035815033702857</v>
+        <v>2.228636730085874</v>
       </c>
       <c r="H11" t="s">
         <v>58</v>
@@ -893,7 +893,7 @@
         <v>57</v>
       </c>
       <c r="G12">
-        <v>2.015739194295643</v>
+        <v>2.15781329499561</v>
       </c>
       <c r="H12" t="s">
         <v>58</v>
@@ -922,7 +922,7 @@
         <v>57</v>
       </c>
       <c r="G13">
-        <v>1.284753493958485</v>
+        <v>1.121832258144104</v>
       </c>
       <c r="H13" t="s">
         <v>58</v>
@@ -951,7 +951,7 @@
         <v>56</v>
       </c>
       <c r="G14">
-        <v>15.04266715042745</v>
+        <v>15.43697013441807</v>
       </c>
       <c r="H14" t="s">
         <v>59</v>
@@ -980,7 +980,7 @@
         <v>57</v>
       </c>
       <c r="G15">
-        <v>11.36325328331444</v>
+        <v>11.09358157116992</v>
       </c>
       <c r="H15" t="s">
         <v>59</v>
@@ -1009,7 +1009,7 @@
         <v>57</v>
       </c>
       <c r="G16">
-        <v>10.28192797181401</v>
+        <v>10.23060859044444</v>
       </c>
       <c r="H16" t="s">
         <v>59</v>
@@ -1038,7 +1038,7 @@
         <v>56</v>
       </c>
       <c r="G17">
-        <v>10.16425277708626</v>
+        <v>10.0348221501642</v>
       </c>
       <c r="H17" t="s">
         <v>59</v>
@@ -1067,7 +1067,7 @@
         <v>57</v>
       </c>
       <c r="G18">
-        <v>9.232871859698882</v>
+        <v>9.495077113351307</v>
       </c>
       <c r="H18" t="s">
         <v>59</v>
@@ -1096,7 +1096,7 @@
         <v>56</v>
       </c>
       <c r="G19">
-        <v>7.274550005288805</v>
+        <v>7.271537858766404</v>
       </c>
       <c r="H19" t="s">
         <v>59</v>
@@ -1113,7 +1113,7 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
         <v>26</v>
@@ -1122,10 +1122,10 @@
         <v>50</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G20">
-        <v>5.284095815019352</v>
+        <v>5.429885939330042</v>
       </c>
       <c r="H20" t="s">
         <v>59</v>
@@ -1142,7 +1142,7 @@
         <v>7</v>
       </c>
       <c r="C21">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
         <v>27</v>
@@ -1151,10 +1151,10 @@
         <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G21">
-        <v>5.117007198824119</v>
+        <v>5.174776003077755</v>
       </c>
       <c r="H21" t="s">
         <v>59</v>
@@ -1171,7 +1171,7 @@
         <v>8</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
         <v>28</v>
@@ -1183,7 +1183,7 @@
         <v>57</v>
       </c>
       <c r="G22">
-        <v>5.092057689109181</v>
+        <v>5.109387050937287</v>
       </c>
       <c r="H22" t="s">
         <v>59</v>
@@ -1212,7 +1212,7 @@
         <v>56</v>
       </c>
       <c r="G23">
-        <v>4.217062184173634</v>
+        <v>4.066289137297956</v>
       </c>
       <c r="H23" t="s">
         <v>59</v>
@@ -1229,7 +1229,7 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
         <v>30</v>
@@ -1241,7 +1241,7 @@
         <v>56</v>
       </c>
       <c r="G24">
-        <v>3.09553860113911</v>
+        <v>3.287022510508467</v>
       </c>
       <c r="H24" t="s">
         <v>59</v>
@@ -1258,7 +1258,7 @@
         <v>11</v>
       </c>
       <c r="C25">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25" t="s">
         <v>31</v>
@@ -1270,7 +1270,7 @@
         <v>56</v>
       </c>
       <c r="G25">
-        <v>3.080972562626874</v>
+        <v>3.121599655266171</v>
       </c>
       <c r="H25" t="s">
         <v>59</v>

</xml_diff>